<commit_message>
Final revisions on tracking script
</commit_message>
<xml_diff>
--- a/Data files/Tracking_codes_Data.xlsx
+++ b/Data files/Tracking_codes_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>URL</t>
   </si>
@@ -52,40 +52,37 @@
     <t>BigInt code expiry</t>
   </si>
   <si>
+    <t>https://www.impact.science/</t>
+  </si>
+  <si>
+    <t>_gat_gtag_UA_140842239_1</t>
+  </si>
+  <si>
+    <t>_ga</t>
+  </si>
+  <si>
+    <t>__ivc</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>2021-08-16 21:21:01 India Standard Time</t>
+  </si>
+  <si>
+    <t>2023-08-16 21:20:01 India Standard Time</t>
+  </si>
+  <si>
     <t>https://lifesciences.cactusglobal.com/</t>
   </si>
   <si>
     <t>_ga_MNGCCS5STP</t>
   </si>
   <si>
-    <t>_ga</t>
-  </si>
-  <si>
-    <t>__ivc</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>2023-08-16 10:58:22 India Standard Time</t>
-  </si>
-  <si>
-    <t>2023-08-16 10:59:09 India Standard Time</t>
-  </si>
-  <si>
-    <t>https://www.impact.science/</t>
-  </si>
-  <si>
-    <t>_gat_gtag_UA_140842239_1</t>
-  </si>
-  <si>
-    <t>2021-08-16 10:59:38 India Standard Time</t>
-  </si>
-  <si>
-    <t>Google analytics script not fired</t>
-  </si>
-  <si>
-    <t>BigInt script not fired</t>
+    <t>2023-08-16 21:20:23 India Standard Time</t>
+  </si>
+  <si>
+    <t>2023-08-16 21:20:24 India Standard Time</t>
   </si>
 </sst>
 </file>
@@ -481,7 +478,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="5">
-        <v>1692163799</v>
+        <v>1692201002</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -580,13 +577,17 @@
         <v>19</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1692201025</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -612,8 +613,8 @@
     <col min="6" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="9.140625" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="20" width="9.140625" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -650,10 +651,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -670,10 +671,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>

</xml_diff>